<commit_message>
updaload test saying hello
</commit_message>
<xml_diff>
--- a/test-resources/data/test_login.xlsx
+++ b/test-resources/data/test_login.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="11711" windowHeight="9167" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9270" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test_data" sheetId="1" r:id="rId1"/>
     <sheet name="test_result" sheetId="2" r:id="rId2"/>
-    <sheet name="test_sayhello" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="23">
   <si>
     <t>Id</t>
   </si>
@@ -85,45 +84,6 @@
   </si>
   <si>
     <t>SUCCESS</t>
-  </si>
-  <si>
-    <t>Fullname</t>
-  </si>
-  <si>
-    <t>Michael Scofield</t>
-  </si>
-  <si>
-    <t>Welcome Michael Scofield</t>
-  </si>
-  <si>
-    <t>Lincoln Burrows</t>
-  </si>
-  <si>
-    <t>Welcome Lincoln Burrows</t>
-  </si>
-  <si>
-    <t>Sara Tancredi</t>
-  </si>
-  <si>
-    <t>Welcome Sara Tancredi</t>
-  </si>
-  <si>
-    <t>Alexander Mahone</t>
-  </si>
-  <si>
-    <t>Welcome Alexander Mahone</t>
-  </si>
-  <si>
-    <t>Fenando Sucre</t>
-  </si>
-  <si>
-    <t>Welcome Fenando Sucre</t>
-  </si>
-  <si>
-    <t>Michael Scott</t>
-  </si>
-  <si>
-    <t>Welcome Michael Scott</t>
   </si>
 </sst>
 </file>
@@ -131,11 +91,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="hh:mm:ss\ dd\-mm\-yyyy"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="hh:mm:ss\ dd\-mm\-yyyy"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -163,12 +123,26 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,7 +152,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -194,31 +168,41 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -231,62 +215,38 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -299,12 +259,96 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -317,25 +361,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,19 +415,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -371,109 +433,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -513,6 +473,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -528,17 +503,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -558,24 +527,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -590,18 +541,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -611,130 +571,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1067,14 +1027,14 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A1" sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="19.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="19.4444444444444" customWidth="1"/>
-    <col min="3" max="3" width="36.7777777777778" customWidth="1"/>
+    <col min="2" max="2" width="19.447619047619" customWidth="1"/>
+    <col min="3" max="3" width="36.7809523809524" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1185,18 +1145,18 @@
   <sheetPr/>
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="7"/>
   <cols>
-    <col min="3" max="3" width="20.2222222222222" customWidth="1"/>
-    <col min="4" max="4" width="22.1111111111111" customWidth="1"/>
-    <col min="5" max="5" width="18.5555555555556" customWidth="1"/>
+    <col min="3" max="3" width="20.2190476190476" customWidth="1"/>
+    <col min="4" max="4" width="22.1142857142857" customWidth="1"/>
+    <col min="5" max="5" width="18.552380952381" customWidth="1"/>
     <col min="6" max="6" width="19.3333333333333" customWidth="1"/>
-    <col min="7" max="7" width="17.7777777777778" customWidth="1"/>
-    <col min="9" max="9" width="35.5555555555556" customWidth="1"/>
+    <col min="7" max="7" width="17.7809523809524" customWidth="1"/>
+    <col min="9" max="9" width="35.552380952381" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1418,81 +1378,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="1"/>
-  <cols>
-    <col min="1" max="1" width="23.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="27.1111111111111" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
upload test saying hello
</commit_message>
<xml_diff>
--- a/test-resources/data/test_login.xlsx
+++ b/test-resources/data/test_login.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9270" activeTab="1"/>
+    <workbookView windowWidth="24345" windowHeight="12510"/>
   </bookViews>
   <sheets>
     <sheet name="test_data" sheetId="1" r:id="rId1"/>
@@ -91,11 +91,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="hh:mm:ss\ dd\-mm\-yyyy"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="hh:mm:ss dd-mm-yyyy"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -123,29 +123,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -166,17 +159,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -184,7 +198,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,6 +209,21 @@
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -206,21 +235,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -228,23 +242,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,187 +259,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,13 +453,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -469,6 +473,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -484,6 +497,32 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -511,52 +550,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -571,140 +571,140 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true" applyNumberFormat="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1026,15 +1026,15 @@
   <sheetPr/>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="19.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="19.447619047619" customWidth="1"/>
-    <col min="3" max="3" width="36.7809523809524" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="19.6666666666667"/>
+    <col min="2" max="2" customWidth="true" width="19.447619047619"/>
+    <col min="3" max="3" customWidth="true" width="36.7809523809524"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1055,7 +1055,7 @@
       <c r="B2">
         <v>123</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1066,7 +1066,7 @@
       <c r="B3">
         <v>123</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1077,7 +1077,7 @@
       <c r="B4">
         <v>123</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1088,7 +1088,7 @@
       <c r="B5">
         <v>123</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1099,7 +1099,7 @@
       <c r="B6">
         <v>123</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1110,7 +1110,7 @@
       <c r="B7">
         <v>123</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1121,7 +1121,7 @@
       <c r="B8">
         <v>123</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1145,19 +1145,19 @@
   <sheetPr/>
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="20.2190476190476" customWidth="1"/>
-    <col min="4" max="4" width="22.1142857142857" customWidth="1"/>
-    <col min="5" max="5" width="18.552380952381" customWidth="1"/>
-    <col min="6" max="6" width="19.3333333333333" customWidth="1"/>
-    <col min="7" max="7" width="17.7809523809524" customWidth="1"/>
-    <col min="9" max="9" width="35.552380952381" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="20.2190476190476"/>
+    <col min="4" max="4" customWidth="true" width="22.1142857142857"/>
+    <col min="5" max="5" customWidth="true" width="18.552380952381"/>
+    <col min="6" max="6" customWidth="true" width="19.3333333333333"/>
+    <col min="7" max="7" customWidth="true" width="17.7809523809524"/>
+    <col min="9" max="9" customWidth="true" width="35.552380952381"/>
+    <col min="10" max="10" customWidth="true" width="14.0"/>
   </cols>
   <sheetData>
     <row r="1" ht="21" customHeight="1" spans="1:10">
@@ -1192,185 +1192,185 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="60" customHeight="1" spans="1:8">
-      <c r="A2" s="1" t="s">
+    <row r="2" ht="60.0" customHeight="true" s="3" customFormat="true">
+      <c r="A2" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s" s="3">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s" s="3">
         <v>20</v>
       </c>
-      <c r="D2" s="1">
-        <v>44894.154025463</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" t="n" s="3">
+        <v>44895.93850538194</v>
+      </c>
+      <c r="E2" t="s" s="3">
         <v>21</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="F2" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="60" customHeight="1" spans="1:8">
-      <c r="A3" s="1" t="s">
+    <row r="3" ht="60.0" customHeight="true" s="3" customFormat="true">
+      <c r="A3" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s" s="3">
         <v>19</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s" s="3">
         <v>20</v>
       </c>
-      <c r="D3" s="1">
-        <v>44894.1541521528</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" t="n" s="3">
+        <v>44895.93857474537</v>
+      </c>
+      <c r="E3" t="s" s="3">
         <v>21</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="F3" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="60" customHeight="1" spans="1:8">
-      <c r="A4" s="1" t="s">
+    <row r="4" ht="60.0" customHeight="true" s="3" customFormat="true">
+      <c r="A4" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s" s="3">
         <v>19</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s" s="3">
         <v>20</v>
       </c>
-      <c r="D4" s="1">
-        <v>44894.1542801157</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4" t="n" s="3">
+        <v>44895.938640925924</v>
+      </c>
+      <c r="E4" t="s" s="3">
         <v>21</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="F4" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" ht="60" customHeight="1" spans="1:8">
-      <c r="A5" s="1" t="s">
+    <row r="5" ht="60.0" customHeight="true" s="3" customFormat="true">
+      <c r="A5" t="s" s="3">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s" s="3">
         <v>19</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s" s="3">
         <v>20</v>
       </c>
-      <c r="D5" s="1">
-        <v>44894.1545943981</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D5" t="n" s="3">
+        <v>44895.93870756945</v>
+      </c>
+      <c r="E5" t="s" s="3">
         <v>21</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="F5" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" ht="60" customHeight="1" spans="1:8">
-      <c r="A6" s="1" t="s">
+    <row r="6" ht="60.0" customHeight="true" s="3" customFormat="true">
+      <c r="A6" t="s" s="3">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s" s="3">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s" s="3">
         <v>20</v>
       </c>
-      <c r="D6" s="1">
-        <v>44894.1547318403</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="D6" t="n" s="3">
+        <v>44895.93896099537</v>
+      </c>
+      <c r="E6" t="s" s="3">
         <v>21</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="F6" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" ht="60" customHeight="1" spans="1:8">
-      <c r="A7" s="1" t="s">
+    <row r="7" ht="60.0" customHeight="true" s="3" customFormat="true">
+      <c r="A7" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s" s="3">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s" s="3">
         <v>20</v>
       </c>
-      <c r="D7" s="1">
-        <v>44894.1548566088</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="D7" t="n" s="3">
+        <v>44895.93921429398</v>
+      </c>
+      <c r="E7" t="s" s="3">
         <v>21</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="1" t="s">
+      <c r="F7" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="H7" t="s" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="8" s="1" customFormat="1" ht="60" customHeight="1" spans="1:8">
-      <c r="A8" s="1" t="s">
+    <row r="8" ht="60.0" customHeight="true" s="3" customFormat="true">
+      <c r="A8" t="s" s="3">
         <v>10</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s" s="3">
         <v>19</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s" s="3">
         <v>20</v>
       </c>
-      <c r="D8" s="1">
-        <v>44894.1551672107</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="D8" t="n" s="3">
+        <v>44895.93946599537</v>
+      </c>
+      <c r="E8" t="s" s="3">
         <v>21</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" t="s" s="3">
         <v>11</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" t="s" s="3">
         <v>11</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" t="s" s="3">
         <v>22</v>
       </c>
     </row>

</xml_diff>